<commit_message>
aded new algoritm QuickSort
</commit_message>
<xml_diff>
--- a/Speed.xlsx
+++ b/Speed.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>SortVibork</t>
   </si>
@@ -34,6 +34,18 @@
   </si>
   <si>
     <t>bubble_sort</t>
+  </si>
+  <si>
+    <t>QuickSort</t>
+  </si>
+  <si>
+    <t>Algoritm</t>
+  </si>
+  <si>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>№</t>
   </si>
 </sst>
 </file>
@@ -43,13 +55,28 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -60,7 +87,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -68,19 +95,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF00FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -355,59 +414,118 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3">
+        <v>9.9802017211913997E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
+        <v>4.98557090759277E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
+      <c r="C4" s="3">
         <v>2.59299278259277E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>4.98557090759277E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="5" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="C5" s="3">
         <v>2.9938936233520501E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="6" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
+      <c r="C6" s="3">
         <v>3.4905672073364202E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="7" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="C7" s="3">
         <v>6.3829421997070299E-2</v>
       </c>
     </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="1"/>
+    </row>
   </sheetData>
+  <sortState ref="B1:C6">
+    <sortCondition ref="C1:C6"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
aded new algoritm SortHeap
</commit_message>
<xml_diff>
--- a/Speed.xlsx
+++ b/Speed.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>SortVibork</t>
   </si>
@@ -46,14 +46,18 @@
   </si>
   <si>
     <t>№</t>
+  </si>
+  <si>
+    <t>SortHeap</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -114,13 +118,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -128,6 +129,15 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -417,7 +427,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,13 +438,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -445,7 +455,7 @@
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="5">
         <v>9.9802017211913997E-4</v>
       </c>
     </row>
@@ -453,11 +463,11 @@
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3">
-        <v>4.98557090759277E-3</v>
+      <c r="B3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="7">
+        <v>3.9899349212646398E-3</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -465,10 +475,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3">
-        <v>2.59299278259277E-2</v>
+        <v>1</v>
+      </c>
+      <c r="C4" s="5">
+        <v>4.98557090759277E-3</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -476,10 +486,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="3">
-        <v>2.9938936233520501E-2</v>
+        <v>0</v>
+      </c>
+      <c r="C5" s="5">
+        <v>2.59299278259277E-2</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -487,10 +497,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="3">
-        <v>3.4905672073364202E-2</v>
+        <v>2</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2.9938936233520501E-2</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -498,9 +508,20 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="5">
+        <v>3.4905672073364202E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C8" s="5">
         <v>6.3829421997070299E-2</v>
       </c>
     </row>
@@ -523,8 +544,8 @@
       <c r="H18" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="B1:C6">
-    <sortCondition ref="C1:C6"/>
+  <sortState ref="B2:C8">
+    <sortCondition ref="C2:C8"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Change speed with and without decorator
</commit_message>
<xml_diff>
--- a/Speed.xlsx
+++ b/Speed.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">№</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">bubble_sort</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Why with decorator the time is small (in all cases)</t>
   </si>
 </sst>
 </file>
@@ -198,13 +201,13 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.15"/>
   </cols>
   <sheetData>
@@ -296,7 +299,14 @@
         <v>0.0638294219970703</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H13" s="1"/>
     </row>

</xml_diff>

<commit_message>
Change Speed.xlsx with comment
</commit_message>
<xml_diff>
--- a/Speed.xlsx
+++ b/Speed.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t xml:space="preserve">Без декоратора</t>
+  </si>
   <si>
     <t xml:space="preserve">№</t>
   </si>
@@ -50,6 +53,9 @@
   </si>
   <si>
     <t xml:space="preserve">bubble_sort</t>
+  </si>
+  <si>
+    <t xml:space="preserve">С декоратором</t>
   </si>
   <si>
     <t xml:space="preserve">Why with decorator the time is small (in all cases)</t>
@@ -64,7 +70,7 @@
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -101,6 +107,14 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -111,7 +125,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -126,6 +140,13 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -152,7 +173,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -179,6 +200,26 @@
     </xf>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -198,10 +239,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -211,104 +252,118 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.15"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" s="5" t="n">
-        <v>0.00099802017211914</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6" t="n">
-        <v>0.00398993492126464</v>
+      <c r="C3" s="5" t="n">
+        <v>0.00099802017211914</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5" t="n">
-        <v>0.00498557090759277</v>
+      <c r="C4" s="6" t="n">
+        <v>0.00398993492126464</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="5" t="n">
-        <v>0.0259299278259277</v>
+        <v>0.00498557090759277</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>0.0299389362335205</v>
+        <v>0.0259299278259277</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="5" t="n">
-        <v>0.0349056720733642</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.0299389362335205</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="5" t="n">
+        <v>0.0349056720733642</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="5" t="n">
         <v>0.0638294219970703</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="1" t="n">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="9"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="11" t="n">
         <v>0.001</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H14" s="1"/>
@@ -324,6 +379,9 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H18" s="1"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H19" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>